<commit_message>
Neues Projekt angelegt wegen visualisierung
</commit_message>
<xml_diff>
--- a/Taskmanagement.xlsx
+++ b/Taskmanagement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kun\Desktop\Uni\Automatisierungstechnik\ProjektaufgabeAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0611C760-891B-4BDA-A83D-32EBD0421C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A24109D-42AE-464E-BDEC-1D4A9EC69D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7FA1E254-1B33-40C8-B6AE-EFE1F4B02A4D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Anforderung</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>Plausibilitätstests entwickeln</t>
+  </si>
+  <si>
+    <t>siehe Datenlexikon</t>
+  </si>
+  <si>
+    <t>Rausfinden wie Text rotieren</t>
   </si>
 </sst>
 </file>
@@ -530,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9E32C3B-A763-4171-98D0-768452F8F394}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,6 +547,7 @@
     <col min="1" max="1" width="43.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -573,6 +580,9 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
       <c r="K2" s="4" t="s">
         <v>4</v>
       </c>
@@ -581,6 +591,9 @@
       <c r="B3" t="s">
         <v>11</v>
       </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
       <c r="K3" s="3" t="s">
         <v>5</v>
       </c>
@@ -589,6 +602,12 @@
       <c r="B4" t="s">
         <v>13</v>
       </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
       <c r="K4" s="2" t="s">
         <v>6</v>
       </c>
@@ -605,11 +624,17 @@
       <c r="B6" t="s">
         <v>16</v>
       </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>17</v>
       </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
@@ -642,30 +667,44 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>23</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>25</v>
+      <c r="D15" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
         <v>28</v>
       </c>
     </row>
@@ -682,7 +721,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="D2:D5 D7:D1048576 D6" xr:uid="{BD9FDE97-7F6A-4810-A886-8AC23400B70E}">
+    <dataValidation type="list" allowBlank="1" sqref="D22:D1048576 D2:D21" xr:uid="{BD9FDE97-7F6A-4810-A886-8AC23400B70E}">
       <formula1>$K$2:$K$5</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
:chart_with_downwards_trend:  Burn Down Chart
</commit_message>
<xml_diff>
--- a/Taskmanagement.xlsx
+++ b/Taskmanagement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kun\Desktop\Uni\Automatisierungstechnik\ProjektaufgabeAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A24109D-42AE-464E-BDEC-1D4A9EC69D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBE8054-395F-4298-AEF2-A92D98A02A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7FA1E254-1B33-40C8-B6AE-EFE1F4B02A4D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t>Anforderung</t>
   </si>
@@ -128,7 +128,34 @@
     <t>siehe Datenlexikon</t>
   </si>
   <si>
-    <t>Rausfinden wie Text rotieren</t>
+    <t>Ghaith</t>
+  </si>
+  <si>
+    <t>Stefan</t>
+  </si>
+  <si>
+    <t>Test Rotieren?</t>
+  </si>
+  <si>
+    <t>Verhalten Steuerelemente bestimmen</t>
+  </si>
+  <si>
+    <t>Steuerelemente einfügen</t>
+  </si>
+  <si>
+    <t>Daten</t>
+  </si>
+  <si>
+    <t>Anzahl</t>
+  </si>
+  <si>
+    <t>Summe Task</t>
+  </si>
+  <si>
+    <t>Task übrig</t>
+  </si>
+  <si>
+    <t>Ideal</t>
   </si>
 </sst>
 </file>
@@ -182,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -190,6 +217,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -229,9 +257,1035 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Burn Down Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Task übrig</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$F$2:$F$22</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>45257</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45257</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45258</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45261</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45320</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$G$2:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-18D2-4702-81A9-96170E4056FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$F$2:$F$22</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>45257</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45257</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45258</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45261</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45320</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$H$2:$H$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-18D2-4702-81A9-96170E4056FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="896382272"/>
+        <c:axId val="905197104"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="896382272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="905197104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="905197104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="896382272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>632460</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Diagramm 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15359E01-BAFB-FFC8-EEBA-A78F240BE9B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EA716592-49C7-4970-845B-5A35992EE658}" name="Tabelle15" displayName="Tabelle15" ref="K1:K4" totalsRowShown="0" dataCellStyle="Standard">
-  <autoFilter ref="K1:K4" xr:uid="{EA716592-49C7-4970-845B-5A35992EE658}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EA716592-49C7-4970-845B-5A35992EE658}" name="Tabelle15" displayName="Tabelle15" ref="L1:L4" totalsRowShown="0" dataCellStyle="Standard">
+  <autoFilter ref="L1:L4" xr:uid="{EA716592-49C7-4970-845B-5A35992EE658}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{7D8F7D5B-1079-49E0-9CAE-8368F0E409DA}" name="Status" dataCellStyle="Standard"/>
   </tableColumns>
@@ -536,10 +1590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9E32C3B-A763-4171-98D0-768452F8F394}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,9 +1602,11 @@
     <col min="2" max="2" width="42" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" customWidth="1"/>
+    <col min="10" max="10" width="1.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -569,11 +1625,29 @@
       <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="S1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -583,22 +1657,56 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="F2" s="5">
+        <v>45257</v>
+      </c>
+      <c r="G2">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2">
+        <f>COUNTA(B2:B26)</f>
+        <v>20</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="S2" s="5">
+        <v>45257</v>
+      </c>
+      <c r="T2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="F3" s="5">
+        <v>45257</v>
+      </c>
+      <c r="G3">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="S3" s="5">
+        <v>45320</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -608,105 +1716,226 @@
       <c r="E4" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="F4" s="5">
+        <v>45258</v>
+      </c>
+      <c r="G4">
+        <v>17</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="S4" s="5"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="S5" s="5"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
       </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="S6" s="5"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>17</v>
       </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="S7" s="5"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="S8" s="5"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="S9" s="5"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="S10" s="5"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="S11" s="5"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="S12" s="5"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="S13" s="5"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="S14" s="5"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="S15" s="5"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="D15" t="s">
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+      <c r="F16" s="5">
+        <v>45261</v>
+      </c>
+      <c r="G16">
+        <v>16</v>
+      </c>
+      <c r="H16">
+        <v>16</v>
+      </c>
+      <c r="S16" s="5"/>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
         <v>25</v>
       </c>
-      <c r="D16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>26</v>
+      <c r="C17" t="s">
+        <v>31</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="S17" s="5"/>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="S18" s="5"/>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="S19" s="5"/>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>28</v>
       </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="S20" s="5"/>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="S21" s="5"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="F22" s="5">
+        <v>45320</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="S22" s="5"/>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="S23" s="5"/>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="S24" s="5"/>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="S25" s="5"/>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="S26" s="5"/>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="S27" s="5"/>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="S28" s="5"/>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="S29" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D1048576">
@@ -720,15 +1949,16 @@
       <formula>NOT(ISERROR(SEARCH("Erledigt",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="D22:D1048576 D2:D21" xr:uid="{BD9FDE97-7F6A-4810-A886-8AC23400B70E}">
-      <formula1>$K$2:$K$5</formula1>
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D1048576" xr:uid="{BD9FDE97-7F6A-4810-A886-8AC23400B70E}">
+      <formula1>$L$2:$L$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>